<commit_message>
Refactor GUI to use files from Core
</commit_message>
<xml_diff>
--- a/support-files/sample_registration.xlsx
+++ b/support-files/sample_registration.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="245">
   <si>
     <t>SID</t>
   </si>
@@ -152,6 +153,603 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Country:</t>
+  </si>
+  <si>
+    <t>Assigned Applicants:</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>the hill school</t>
+  </si>
+  <si>
+    <t>new zealand</t>
+  </si>
+  <si>
+    <t>flordia pine crest</t>
+  </si>
+  <si>
+    <t>canada</t>
+  </si>
+  <si>
+    <t>the taft school</t>
+  </si>
+  <si>
+    <t>united states of america</t>
+  </si>
+  <si>
+    <t>horrace mann</t>
+  </si>
+  <si>
+    <t>antigua and barbuda</t>
+  </si>
+  <si>
+    <t>the landon school</t>
+  </si>
+  <si>
+    <t>bahamas</t>
+  </si>
+  <si>
+    <t>barbados</t>
+  </si>
+  <si>
+    <t>cuba</t>
+  </si>
+  <si>
+    <t>dominica</t>
+  </si>
+  <si>
+    <t>dominican republic</t>
+  </si>
+  <si>
+    <t>grenada</t>
+  </si>
+  <si>
+    <t>haiti</t>
+  </si>
+  <si>
+    <t>jamaica</t>
+  </si>
+  <si>
+    <t>saint kitts and nevis</t>
+  </si>
+  <si>
+    <t>saint lucia</t>
+  </si>
+  <si>
+    <t>saint vincent and the grenadines</t>
+  </si>
+  <si>
+    <t>trinidad and tobago</t>
+  </si>
+  <si>
+    <t>angola</t>
+  </si>
+  <si>
+    <t>cameroon</t>
+  </si>
+  <si>
+    <t>central african republic</t>
+  </si>
+  <si>
+    <t>chad</t>
+  </si>
+  <si>
+    <t>congo (republic of the)</t>
+  </si>
+  <si>
+    <t>democratic republic of the congo</t>
+  </si>
+  <si>
+    <t>equatorial guinea</t>
+  </si>
+  <si>
+    <t>gabon</t>
+  </si>
+  <si>
+    <t>sao tome and principe</t>
+  </si>
+  <si>
+    <t>belize</t>
+  </si>
+  <si>
+    <t>costa rica</t>
+  </si>
+  <si>
+    <t>el salvador</t>
+  </si>
+  <si>
+    <t>guatemala</t>
+  </si>
+  <si>
+    <t>honduras</t>
+  </si>
+  <si>
+    <t>mexico</t>
+  </si>
+  <si>
+    <t>nicaragua</t>
+  </si>
+  <si>
+    <t>panama</t>
+  </si>
+  <si>
+    <t>kazakhstan</t>
+  </si>
+  <si>
+    <t>kyrgyzstan</t>
+  </si>
+  <si>
+    <t>tajikistan</t>
+  </si>
+  <si>
+    <t>turkmenistan</t>
+  </si>
+  <si>
+    <t>uzbekistan</t>
+  </si>
+  <si>
+    <t>burundi</t>
+  </si>
+  <si>
+    <t>comoros</t>
+  </si>
+  <si>
+    <t>djibouti</t>
+  </si>
+  <si>
+    <t>eritrea</t>
+  </si>
+  <si>
+    <t>ethiopia</t>
+  </si>
+  <si>
+    <t>kenya</t>
+  </si>
+  <si>
+    <t>madagascar</t>
+  </si>
+  <si>
+    <t>malawi</t>
+  </si>
+  <si>
+    <t>mauritius</t>
+  </si>
+  <si>
+    <t>mozambique</t>
+  </si>
+  <si>
+    <t>rwanda</t>
+  </si>
+  <si>
+    <t>seychelles</t>
+  </si>
+  <si>
+    <t>somalia</t>
+  </si>
+  <si>
+    <t>south sudan</t>
+  </si>
+  <si>
+    <t>uganda</t>
+  </si>
+  <si>
+    <t>united republic of tanzania</t>
+  </si>
+  <si>
+    <t>zambia</t>
+  </si>
+  <si>
+    <t>zimbabwe</t>
+  </si>
+  <si>
+    <t>china</t>
+  </si>
+  <si>
+    <t>democratic people's republic of korea</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>mongolia</t>
+  </si>
+  <si>
+    <t>republic of korea</t>
+  </si>
+  <si>
+    <t>belarus</t>
+  </si>
+  <si>
+    <t>bulgaria</t>
+  </si>
+  <si>
+    <t>czech republic</t>
+  </si>
+  <si>
+    <t>hungary</t>
+  </si>
+  <si>
+    <t>poland</t>
+  </si>
+  <si>
+    <t>republic of moldova</t>
+  </si>
+  <si>
+    <t>republic of serbia</t>
+  </si>
+  <si>
+    <t>romania</t>
+  </si>
+  <si>
+    <t>russian federation</t>
+  </si>
+  <si>
+    <t>slovakia</t>
+  </si>
+  <si>
+    <t>ukraine</t>
+  </si>
+  <si>
+    <t>armenia</t>
+  </si>
+  <si>
+    <t>azerbaijan</t>
+  </si>
+  <si>
+    <t>bahrain</t>
+  </si>
+  <si>
+    <t>cyprus</t>
+  </si>
+  <si>
+    <t>georgia</t>
+  </si>
+  <si>
+    <t>iraq</t>
+  </si>
+  <si>
+    <t>israel</t>
+  </si>
+  <si>
+    <t>jordan</t>
+  </si>
+  <si>
+    <t>kuwait</t>
+  </si>
+  <si>
+    <t>lebanon</t>
+  </si>
+  <si>
+    <t>oman</t>
+  </si>
+  <si>
+    <t>qatar</t>
+  </si>
+  <si>
+    <t>saudi arabia</t>
+  </si>
+  <si>
+    <t>syrian arab republic</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>yemen</t>
+  </si>
+  <si>
+    <t>algeria</t>
+  </si>
+  <si>
+    <t>egypt</t>
+  </si>
+  <si>
+    <t>libya</t>
+  </si>
+  <si>
+    <t>morocco</t>
+  </si>
+  <si>
+    <t>sudan</t>
+  </si>
+  <si>
+    <t>tunisia</t>
+  </si>
+  <si>
+    <t>denmark</t>
+  </si>
+  <si>
+    <t>estonia</t>
+  </si>
+  <si>
+    <t>finland</t>
+  </si>
+  <si>
+    <t>iceland</t>
+  </si>
+  <si>
+    <t>ireland</t>
+  </si>
+  <si>
+    <t>latvia</t>
+  </si>
+  <si>
+    <t>lithuania</t>
+  </si>
+  <si>
+    <t>norway</t>
+  </si>
+  <si>
+    <t>sweden</t>
+  </si>
+  <si>
+    <t>fiji</t>
+  </si>
+  <si>
+    <t>papua new guinea</t>
+  </si>
+  <si>
+    <t>solomon islands</t>
+  </si>
+  <si>
+    <t>vanuatu</t>
+  </si>
+  <si>
+    <t>venezuela</t>
+  </si>
+  <si>
+    <t>kiribati</t>
+  </si>
+  <si>
+    <t>marshall islands</t>
+  </si>
+  <si>
+    <t>nauru</t>
+  </si>
+  <si>
+    <t>palau</t>
+  </si>
+  <si>
+    <t>samoa</t>
+  </si>
+  <si>
+    <t>tonga</t>
+  </si>
+  <si>
+    <t>tuvalu</t>
+  </si>
+  <si>
+    <t>argentina</t>
+  </si>
+  <si>
+    <t>bolivia</t>
+  </si>
+  <si>
+    <t>brazil</t>
+  </si>
+  <si>
+    <t>chile</t>
+  </si>
+  <si>
+    <t>colombia</t>
+  </si>
+  <si>
+    <t>ecuador</t>
+  </si>
+  <si>
+    <t>guyana</t>
+  </si>
+  <si>
+    <t>federated states of micronesia</t>
+  </si>
+  <si>
+    <t>paraguay</t>
+  </si>
+  <si>
+    <t>peru</t>
+  </si>
+  <si>
+    <t>suriname</t>
+  </si>
+  <si>
+    <t>uruguay</t>
+  </si>
+  <si>
+    <t>brunei darussalam</t>
+  </si>
+  <si>
+    <t>cambodia</t>
+  </si>
+  <si>
+    <t>indonesia</t>
+  </si>
+  <si>
+    <t>iran</t>
+  </si>
+  <si>
+    <t>lao people's democratic republic</t>
+  </si>
+  <si>
+    <t>malaysia</t>
+  </si>
+  <si>
+    <t>myanmar</t>
+  </si>
+  <si>
+    <t>philippines</t>
+  </si>
+  <si>
+    <t>singapore</t>
+  </si>
+  <si>
+    <t>thailand</t>
+  </si>
+  <si>
+    <t>timor-leste</t>
+  </si>
+  <si>
+    <t>viet nam</t>
+  </si>
+  <si>
+    <t>botswana</t>
+  </si>
+  <si>
+    <t>lesotho</t>
+  </si>
+  <si>
+    <t>namibia</t>
+  </si>
+  <si>
+    <t>south africa</t>
+  </si>
+  <si>
+    <t>swaziland</t>
+  </si>
+  <si>
+    <t>afghanistan</t>
+  </si>
+  <si>
+    <t>bangladesh</t>
+  </si>
+  <si>
+    <t>bhutan</t>
+  </si>
+  <si>
+    <t>india</t>
+  </si>
+  <si>
+    <t>maldives</t>
+  </si>
+  <si>
+    <t>nepal</t>
+  </si>
+  <si>
+    <t>pakistan</t>
+  </si>
+  <si>
+    <t>sri lanka</t>
+  </si>
+  <si>
+    <t>albania</t>
+  </si>
+  <si>
+    <t>andorra</t>
+  </si>
+  <si>
+    <t>bosnia and herzegovina</t>
+  </si>
+  <si>
+    <t>croatia</t>
+  </si>
+  <si>
+    <t>greece</t>
+  </si>
+  <si>
+    <t>italy</t>
+  </si>
+  <si>
+    <t>malta</t>
+  </si>
+  <si>
+    <t>montenegro</t>
+  </si>
+  <si>
+    <t>portugal</t>
+  </si>
+  <si>
+    <t>san marino</t>
+  </si>
+  <si>
+    <t>slovenia</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>the former yugoslav republic of macedonia</t>
+  </si>
+  <si>
+    <t>benin</t>
+  </si>
+  <si>
+    <t>burkina faso</t>
+  </si>
+  <si>
+    <t>cape verde</t>
+  </si>
+  <si>
+    <t>cote d'ivoire</t>
+  </si>
+  <si>
+    <t>gambia</t>
+  </si>
+  <si>
+    <t>ghana</t>
+  </si>
+  <si>
+    <t>guinea</t>
+  </si>
+  <si>
+    <t>guinea-bissau</t>
+  </si>
+  <si>
+    <t>liberia</t>
+  </si>
+  <si>
+    <t>mali</t>
+  </si>
+  <si>
+    <t>mauritania</t>
+  </si>
+  <si>
+    <t>niger</t>
+  </si>
+  <si>
+    <t>nigeria</t>
+  </si>
+  <si>
+    <t>senegal</t>
+  </si>
+  <si>
+    <t>sierra leone</t>
+  </si>
+  <si>
+    <t>togo</t>
+  </si>
+  <si>
+    <t>united arab emirates</t>
+  </si>
+  <si>
+    <t>united kingdom</t>
+  </si>
+  <si>
+    <t>austria</t>
+  </si>
+  <si>
+    <t>belgium</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>germany</t>
+  </si>
+  <si>
+    <t>liechtenstein</t>
+  </si>
+  <si>
+    <t>luxembourg</t>
+  </si>
+  <si>
+    <t>monaco</t>
+  </si>
+  <si>
+    <t>netherlands</t>
   </si>
 </sst>
 </file>
@@ -534,7 +1132,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -834,4 +1434,1000 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B193"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" t="s">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>